<commit_message>
fix: Rename MetaData XLS tab
</commit_message>
<xml_diff>
--- a/_imports/MFFContent.xlsx
+++ b/_imports/MFFContent.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbraga\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmabonzo/dev/ep/mff/_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DA132D4-9E5A-417E-ACBD-D883F4DEAC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD41C8D-E489-6A41-B0BF-E0A31B78AFA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MetaData" sheetId="2" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId1"/>
     <sheet name="Homepage" sheetId="3" r:id="rId2"/>
     <sheet name="Why it matters" sheetId="1" r:id="rId3"/>
     <sheet name="How it works" sheetId="24" r:id="rId4"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_GoBack">Homepage!$B$19</definedName>
   </definedNames>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,10 +35,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -8183,7 +8183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10913,21 +10913,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="12" width="8.5703125" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" customWidth="1"/>
-    <col min="14" max="25" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+    <col min="3" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="7.5" customWidth="1"/>
+    <col min="14" max="25" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -11019,7 +11019,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>30</v>
       </c>
@@ -11101,7 +11101,7 @@
       <c r="AC2" s="28"/>
       <c r="AD2" s="28"/>
     </row>
-    <row r="3" spans="1:30" ht="15.75">
+    <row r="3" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>53</v>
       </c>
@@ -11137,7 +11137,7 @@
       <c r="AC3" s="53"/>
       <c r="AD3" s="53"/>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>55</v>
       </c>
@@ -11173,7 +11173,7 @@
       <c r="AC4" s="27"/>
       <c r="AD4" s="27"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>57</v>
       </c>
@@ -11209,7 +11209,7 @@
       <c r="AC5" s="27"/>
       <c r="AD5" s="27"/>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>59</v>
       </c>
@@ -11245,7 +11245,7 @@
       <c r="AC6" s="27"/>
       <c r="AD6" s="27"/>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>61</v>
       </c>
@@ -11327,7 +11327,7 @@
       <c r="AC7" s="27"/>
       <c r="AD7" s="27"/>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>86</v>
       </c>
@@ -11409,7 +11409,7 @@
       <c r="AC8" s="27"/>
       <c r="AD8" s="27"/>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>110</v>
       </c>
@@ -11491,7 +11491,7 @@
       <c r="AC9" s="27"/>
       <c r="AD9" s="27"/>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>135</v>
       </c>
@@ -11573,7 +11573,7 @@
       <c r="AC10" s="27"/>
       <c r="AD10" s="27"/>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>160</v>
       </c>
@@ -11655,7 +11655,7 @@
       <c r="AC11" s="27"/>
       <c r="AD11" s="27"/>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>175</v>
       </c>
@@ -11737,7 +11737,7 @@
       <c r="AC12" s="27"/>
       <c r="AD12" s="27"/>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>200</v>
       </c>
@@ -11819,7 +11819,7 @@
       <c r="AC13" s="27"/>
       <c r="AD13" s="27"/>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>225</v>
       </c>
@@ -11901,7 +11901,7 @@
       <c r="AC14" s="27"/>
       <c r="AD14" s="27"/>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>250</v>
       </c>
@@ -11983,7 +11983,7 @@
       <c r="AC15" s="27"/>
       <c r="AD15" s="27"/>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>275</v>
       </c>
@@ -12065,7 +12065,7 @@
       <c r="AC16" s="27"/>
       <c r="AD16" s="27"/>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>299</v>
       </c>
@@ -12147,7 +12147,7 @@
       <c r="AC17" s="27"/>
       <c r="AD17" s="27"/>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>324</v>
       </c>
@@ -12229,7 +12229,7 @@
       <c r="AC18" s="27"/>
       <c r="AD18" s="27"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>349</v>
       </c>
@@ -12311,7 +12311,7 @@
       <c r="AC19" s="27"/>
       <c r="AD19" s="27"/>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>374</v>
       </c>
@@ -12393,7 +12393,7 @@
       <c r="AC20" s="27"/>
       <c r="AD20" s="27"/>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>399</v>
       </c>
@@ -12475,7 +12475,7 @@
       <c r="AC21" s="27"/>
       <c r="AD21" s="27"/>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>424</v>
       </c>
@@ -12557,7 +12557,7 @@
       <c r="AC22" s="27"/>
       <c r="AD22" s="27"/>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>449</v>
       </c>
@@ -12639,7 +12639,7 @@
       <c r="AC23" s="27"/>
       <c r="AD23" s="27"/>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>474</v>
       </c>
@@ -12721,7 +12721,7 @@
       <c r="AC24" s="27"/>
       <c r="AD24" s="27"/>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>499</v>
       </c>
@@ -12803,7 +12803,7 @@
       <c r="AC25" s="27"/>
       <c r="AD25" s="27"/>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>524</v>
       </c>
@@ -12885,7 +12885,7 @@
       <c r="AC26" s="27"/>
       <c r="AD26" s="27"/>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>549</v>
       </c>
@@ -12967,7 +12967,7 @@
       <c r="AC27" s="27"/>
       <c r="AD27" s="27"/>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>574</v>
       </c>
@@ -13049,7 +13049,7 @@
       <c r="AC28" s="27"/>
       <c r="AD28" s="27"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>599</v>
       </c>
@@ -13131,7 +13131,7 @@
       <c r="AC29" s="27"/>
       <c r="AD29" s="27"/>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>624</v>
       </c>
@@ -13213,7 +13213,7 @@
       <c r="AC30" s="27"/>
       <c r="AD30" s="27"/>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
         <v>647</v>
       </c>
@@ -13295,7 +13295,7 @@
       <c r="AC31" s="53"/>
       <c r="AD31" s="53"/>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>672</v>
       </c>
@@ -13377,7 +13377,7 @@
       <c r="AC32" s="27"/>
       <c r="AD32" s="27"/>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>689</v>
       </c>
@@ -13459,7 +13459,7 @@
       <c r="AC33" s="27"/>
       <c r="AD33" s="27"/>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>714</v>
       </c>
@@ -13541,7 +13541,7 @@
       <c r="AC34" s="27"/>
       <c r="AD34" s="27"/>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>739</v>
       </c>
@@ -13623,7 +13623,7 @@
       <c r="AC35" s="27"/>
       <c r="AD35" s="27"/>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
         <v>764</v>
       </c>
@@ -13659,7 +13659,7 @@
       <c r="AC36" s="27"/>
       <c r="AD36" s="27"/>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>766</v>
       </c>
@@ -13741,7 +13741,7 @@
       <c r="AC37" s="27"/>
       <c r="AD37" s="27"/>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
         <v>791</v>
       </c>
@@ -13823,7 +13823,7 @@
       <c r="AC38" s="27"/>
       <c r="AD38" s="27"/>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
         <v>816</v>
       </c>
@@ -13857,7 +13857,7 @@
       <c r="AC39" s="27"/>
       <c r="AD39" s="27"/>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>817</v>
       </c>
@@ -13939,7 +13939,7 @@
       <c r="AC40" s="27"/>
       <c r="AD40" s="27"/>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
         <v>838</v>
       </c>
@@ -14021,7 +14021,7 @@
       <c r="AC41" s="27"/>
       <c r="AD41" s="27"/>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
         <v>863</v>
       </c>
@@ -14103,7 +14103,7 @@
       <c r="AC42" s="27"/>
       <c r="AD42" s="27"/>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>888</v>
       </c>
@@ -14185,7 +14185,7 @@
       <c r="AC43" s="27"/>
       <c r="AD43" s="27"/>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>913</v>
       </c>
@@ -14267,7 +14267,7 @@
       <c r="AC44" s="27"/>
       <c r="AD44" s="27"/>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>938</v>
       </c>
@@ -14349,7 +14349,7 @@
       <c r="AC45" s="27"/>
       <c r="AD45" s="27"/>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>963</v>
       </c>
@@ -14431,7 +14431,7 @@
       <c r="AC46" s="27"/>
       <c r="AD46" s="27"/>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>966</v>
       </c>
@@ -14445,7 +14445,7 @@
       <c r="AC47" s="27"/>
       <c r="AD47" s="27"/>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>968</v>
       </c>
@@ -14527,7 +14527,7 @@
       <c r="AC48" s="27"/>
       <c r="AD48" s="27"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>988</v>
       </c>
@@ -14609,7 +14609,7 @@
       <c r="AC49" s="27"/>
       <c r="AD49" s="27"/>
     </row>
-    <row r="50" spans="1:31" s="22" customFormat="1">
+    <row r="50" spans="1:31" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>1013</v>
       </c>
@@ -14687,7 +14687,7 @@
       </c>
       <c r="AE50" s="53"/>
     </row>
-    <row r="51" spans="1:31" s="22" customFormat="1">
+    <row r="51" spans="1:31" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
         <v>1038</v>
       </c>
@@ -14765,7 +14765,7 @@
       </c>
       <c r="AE51" s="53"/>
     </row>
-    <row r="52" spans="1:31" s="22" customFormat="1">
+    <row r="52" spans="1:31" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
         <v>1063</v>
       </c>
@@ -14843,7 +14843,7 @@
       </c>
       <c r="AE52" s="53"/>
     </row>
-    <row r="53" spans="1:31" s="22" customFormat="1" ht="15.75">
+    <row r="53" spans="1:31" s="22" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="30" t="s">
         <v>1088</v>
       </c>
@@ -14921,7 +14921,7 @@
       </c>
       <c r="AE53" s="53"/>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A54" s="30" t="s">
         <v>1113</v>
       </c>
@@ -14934,7 +14934,7 @@
       <c r="AC54" s="27"/>
       <c r="AD54" s="27"/>
     </row>
-    <row r="55" spans="1:31" ht="15.75">
+    <row r="55" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="30" t="s">
         <v>1115</v>
       </c>
@@ -15016,7 +15016,7 @@
       <c r="AC55" s="27"/>
       <c r="AD55" s="27"/>
     </row>
-    <row r="56" spans="1:31" ht="15.75">
+    <row r="56" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="30" t="s">
         <v>1133</v>
       </c>
@@ -15098,7 +15098,7 @@
       <c r="AC56" s="27"/>
       <c r="AD56" s="27"/>
     </row>
-    <row r="57" spans="1:31" ht="15.75">
+    <row r="57" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="30" t="s">
         <v>1154</v>
       </c>
@@ -15180,7 +15180,7 @@
       <c r="AC57" s="27"/>
       <c r="AD57" s="27"/>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A58" s="30" t="s">
         <v>1175</v>
       </c>
@@ -15262,7 +15262,7 @@
       <c r="AC58" s="27"/>
       <c r="AD58" s="27"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A59" s="30" t="s">
         <v>1200</v>
       </c>
@@ -15344,7 +15344,7 @@
       <c r="AC59" s="27"/>
       <c r="AD59" s="27"/>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A60" s="54" t="s">
         <v>1225</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
         <v>1250</v>
       </c>
@@ -15528,7 +15528,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1275</v>
       </c>
@@ -15605,7 +15605,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1277</v>
       </c>
@@ -15860,19 +15860,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A48" sqref="A48:A49"/>
-      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="3" customWidth="1"/>
-    <col min="3" max="25" width="6.140625" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="10.28515625" style="3"/>
+    <col min="1" max="1" width="37.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="3" customWidth="1"/>
+    <col min="3" max="25" width="6.1640625" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="10.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -15949,7 +15949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1279</v>
       </c>
@@ -15980,7 +15980,7 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1281</v>
       </c>
@@ -15989,10 +15989,10 @@
       </c>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1283</v>
       </c>
@@ -16000,7 +16000,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1285</v>
       </c>
@@ -16008,7 +16008,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="114">
+    <row r="8" spans="1:25" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1287</v>
       </c>
@@ -16016,7 +16016,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="12" customFormat="1">
+    <row r="10" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>1289</v>
       </c>
@@ -16024,7 +16024,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="12" customFormat="1">
+    <row r="11" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>1290</v>
       </c>
@@ -16101,7 +16101,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="12" customFormat="1" ht="42.75">
+    <row r="12" spans="1:25" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>1315</v>
       </c>
@@ -16109,10 +16109,10 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="13" spans="1:25" s="12" customFormat="1">
+    <row r="13" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="14"/>
     </row>
-    <row r="14" spans="1:25" s="12" customFormat="1">
+    <row r="14" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>1289</v>
       </c>
@@ -16143,7 +16143,7 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" s="12" customFormat="1">
+    <row r="15" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>1290</v>
       </c>
@@ -16220,7 +16220,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="12" customFormat="1" ht="42.75">
+    <row r="16" spans="1:25" s="12" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>1315</v>
       </c>
@@ -16228,10 +16228,10 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="12" customFormat="1">
+    <row r="17" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="14"/>
     </row>
-    <row r="18" spans="1:26" s="43" customFormat="1" ht="15">
+    <row r="18" spans="1:26" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>1289</v>
       </c>
@@ -16263,7 +16263,7 @@
       <c r="Y18" s="69"/>
       <c r="Z18" s="69"/>
     </row>
-    <row r="19" spans="1:26" s="44" customFormat="1" ht="15">
+    <row r="19" spans="1:26" s="44" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>1290</v>
       </c>
@@ -16341,7 +16341,7 @@
       </c>
       <c r="Z19" s="69"/>
     </row>
-    <row r="20" spans="1:26" s="44" customFormat="1" ht="45.75">
+    <row r="20" spans="1:26" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>1315</v>
       </c>
@@ -16373,7 +16373,7 @@
       <c r="Y20" s="10"/>
       <c r="Z20" s="69"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B21" s="14"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -16399,7 +16399,7 @@
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
     </row>
-    <row r="22" spans="1:26" ht="15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>1289</v>
       </c>
@@ -16430,7 +16430,7 @@
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
     </row>
-    <row r="23" spans="1:26" ht="15">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>1290</v>
       </c>
@@ -16507,7 +16507,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="30.75">
+    <row r="24" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>1315</v>
       </c>
@@ -16538,10 +16538,10 @@
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:26" s="34" customFormat="1">
+    <row r="26" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
         <v>1394</v>
       </c>
@@ -16570,7 +16570,7 @@
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
     </row>
-    <row r="27" spans="1:26" s="34" customFormat="1">
+    <row r="27" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>1395</v>
       </c>
@@ -16599,7 +16599,7 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
     </row>
-    <row r="28" spans="1:26" s="34" customFormat="1">
+    <row r="28" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="15"/>
       <c r="C28" s="3"/>
@@ -16626,7 +16626,7 @@
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
     </row>
-    <row r="29" spans="1:26" s="34" customFormat="1">
+    <row r="29" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>1396</v>
       </c>
@@ -16657,7 +16657,7 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
     </row>
-    <row r="30" spans="1:26" s="34" customFormat="1">
+    <row r="30" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>1398</v>
       </c>
@@ -16688,7 +16688,7 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
     </row>
-    <row r="31" spans="1:26" s="34" customFormat="1" ht="28.5">
+    <row r="31" spans="1:26" s="34" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>1400</v>
       </c>
@@ -16719,7 +16719,7 @@
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
     </row>
-    <row r="32" spans="1:26" s="34" customFormat="1">
+    <row r="32" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>1398</v>
       </c>
@@ -16750,7 +16750,7 @@
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
     </row>
-    <row r="33" spans="1:26" s="34" customFormat="1" ht="28.5">
+    <row r="33" spans="1:26" s="34" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>1400</v>
       </c>
@@ -16781,7 +16781,7 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34" spans="1:26" s="34" customFormat="1">
+    <row r="34" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>1398</v>
       </c>
@@ -16812,7 +16812,7 @@
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
     </row>
-    <row r="35" spans="1:26" s="34" customFormat="1" ht="42.75">
+    <row r="35" spans="1:26" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>1400</v>
       </c>
@@ -16843,7 +16843,7 @@
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36" spans="1:26" s="34" customFormat="1">
+    <row r="36" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="15"/>
       <c r="C36" s="3"/>
@@ -16870,7 +16870,7 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37" spans="1:26" s="34" customFormat="1">
+    <row r="37" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>1406</v>
       </c>
@@ -16901,7 +16901,7 @@
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
     </row>
-    <row r="38" spans="1:26" s="34" customFormat="1">
+    <row r="38" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>1407</v>
       </c>
@@ -16932,7 +16932,7 @@
       <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
     </row>
-    <row r="39" spans="1:26" s="34" customFormat="1">
+    <row r="39" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>1409</v>
       </c>
@@ -16961,7 +16961,7 @@
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
     </row>
-    <row r="40" spans="1:26" s="34" customFormat="1">
+    <row r="40" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="15"/>
       <c r="C40" s="3"/>
@@ -16988,7 +16988,7 @@
       <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
     </row>
-    <row r="41" spans="1:26" s="34" customFormat="1">
+    <row r="41" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>1410</v>
       </c>
@@ -17019,7 +17019,7 @@
       <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
     </row>
-    <row r="42" spans="1:26" s="34" customFormat="1">
+    <row r="42" spans="1:26" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>1412</v>
       </c>
@@ -17050,7 +17050,7 @@
       <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
     </row>
-    <row r="43" spans="1:26" s="34" customFormat="1">
+    <row r="43" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>1414</v>
       </c>
@@ -17127,7 +17127,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="34" customFormat="1">
+    <row r="44" spans="1:26" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>1412</v>
       </c>
@@ -17158,7 +17158,7 @@
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
     </row>
-    <row r="45" spans="1:26" s="34" customFormat="1">
+    <row r="45" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>1414</v>
       </c>
@@ -17235,7 +17235,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="46" spans="1:26" s="34" customFormat="1" ht="28.5">
+    <row r="46" spans="1:26" s="34" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>1412</v>
       </c>
@@ -17266,7 +17266,7 @@
       <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
     </row>
-    <row r="47" spans="1:26" s="33" customFormat="1" ht="15">
+    <row r="47" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>1414</v>
       </c>
@@ -17343,7 +17343,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="48" spans="1:26" s="34" customFormat="1" ht="30.75">
+    <row r="48" spans="1:26" s="34" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>1412</v>
       </c>
@@ -17355,7 +17355,7 @@
       <c r="Y48" s="45"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" spans="1:25" s="33" customFormat="1" ht="15">
+    <row r="49" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>1414</v>
       </c>
@@ -17432,7 +17432,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="12" customFormat="1">
+    <row r="50" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="32"/>
       <c r="B50" s="17"/>
       <c r="C50" s="2"/>
@@ -17459,7 +17459,7 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" s="12" customFormat="1">
+    <row r="51" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="33"/>
       <c r="B51" s="33"/>
       <c r="C51" s="33"/>
@@ -17486,7 +17486,7 @@
       <c r="X51" s="33"/>
       <c r="Y51" s="33"/>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="33"/>
       <c r="B52" s="33" t="s">
         <v>1514</v>
@@ -17647,17 +17647,17 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="3" customWidth="1"/>
-    <col min="3" max="23" width="8.28515625" style="3"/>
-    <col min="24" max="24" width="10.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="7.5703125" style="7" customWidth="1"/>
-    <col min="26" max="16384" width="8.28515625" style="3"/>
+    <col min="2" max="2" width="40.33203125" style="3" customWidth="1"/>
+    <col min="3" max="23" width="8.33203125" style="3"/>
+    <col min="24" max="24" width="10.1640625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="7.5" style="7" customWidth="1"/>
+    <col min="26" max="16384" width="8.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75" customHeight="1">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -17734,7 +17734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="12.75" customHeight="1">
+    <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1279</v>
       </c>
@@ -17743,7 +17743,7 @@
       </c>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3" spans="1:25" ht="12.75" customHeight="1">
+    <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1281</v>
       </c>
@@ -17751,10 +17751,10 @@
         <v>1516</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="12.75" customHeight="1">
+    <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
     </row>
-    <row r="5" spans="1:25" ht="12.75" customHeight="1">
+    <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1517</v>
       </c>
@@ -17762,7 +17762,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="12.75" customHeight="1">
+    <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1518</v>
       </c>
@@ -17770,7 +17770,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1520</v>
       </c>
@@ -17778,7 +17778,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1521</v>
       </c>
@@ -17786,7 +17786,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1522</v>
       </c>
@@ -17817,7 +17817,7 @@
       <c r="X10" s="35"/>
       <c r="Y10" s="16"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1520</v>
       </c>
@@ -17825,7 +17825,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1521</v>
       </c>
@@ -17834,7 +17834,7 @@
       </c>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1522</v>
       </c>
@@ -17889,16 +17889,16 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="3" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="3" customWidth="1"/>
     <col min="4" max="25" width="8" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="8.28515625" style="3"/>
+    <col min="26" max="16384" width="8.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75" customHeight="1">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -17975,7 +17975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="12.75" customHeight="1">
+    <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1279</v>
       </c>
@@ -17983,7 +17983,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="12.75" customHeight="1">
+    <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1281</v>
       </c>
@@ -17991,10 +17991,10 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="12.75" customHeight="1">
+    <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
     </row>
-    <row r="5" spans="1:25" ht="12.75" customHeight="1">
+    <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1517</v>
       </c>
@@ -18009,7 +18009,7 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="1:25" ht="75.400000000000006" customHeight="1">
+    <row r="6" spans="1:25" ht="75.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1518</v>
       </c>
@@ -18039,7 +18039,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18047,7 +18047,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1521</v>
       </c>
@@ -18078,7 +18078,7 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1522</v>
       </c>
@@ -18109,7 +18109,7 @@
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1521</v>
       </c>
@@ -18147,7 +18147,7 @@
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1522</v>
       </c>
@@ -18237,16 +18237,16 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="3" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="3" customWidth="1"/>
     <col min="4" max="25" width="8" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="8.28515625" style="3"/>
+    <col min="26" max="16384" width="8.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75" customHeight="1">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -18323,7 +18323,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="12.75" customHeight="1">
+    <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1279</v>
       </c>
@@ -18331,7 +18331,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="12.75" customHeight="1">
+    <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1281</v>
       </c>
@@ -18339,10 +18339,10 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="12.75" customHeight="1">
+    <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
     </row>
-    <row r="5" spans="1:25" ht="12.75" customHeight="1">
+    <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1517</v>
       </c>
@@ -18367,7 +18367,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:25" ht="63.75" customHeight="1">
+    <row r="6" spans="1:25" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1518</v>
       </c>
@@ -18398,7 +18398,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18406,7 +18406,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1521</v>
       </c>
@@ -18437,7 +18437,7 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1522</v>
       </c>
@@ -18468,7 +18468,7 @@
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18476,7 +18476,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1521</v>
       </c>
@@ -18506,7 +18506,7 @@
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1522</v>
       </c>
@@ -18596,21 +18596,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76234A24-E978-4A99-9F21-44A727933508}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="3" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="3" customWidth="1"/>
     <col min="4" max="25" width="8" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="8.28515625" style="3"/>
+    <col min="26" max="16384" width="8.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75" customHeight="1">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -18687,7 +18687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="12.75" customHeight="1">
+    <row r="2" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1279</v>
       </c>
@@ -18695,7 +18695,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="12.75" customHeight="1">
+    <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1281</v>
       </c>
@@ -18703,10 +18703,10 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="12.75" customHeight="1">
+    <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
     </row>
-    <row r="5" spans="1:25" ht="12.75" customHeight="1">
+    <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1517</v>
       </c>
@@ -18731,7 +18731,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:25" ht="63.75" customHeight="1">
+    <row r="6" spans="1:25" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1518</v>
       </c>
@@ -18762,7 +18762,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1">
+    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18770,7 +18770,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" customHeight="1">
+    <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1521</v>
       </c>
@@ -18801,7 +18801,7 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" customHeight="1">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1522</v>
       </c>
@@ -18832,7 +18832,7 @@
       <c r="X10" s="16"/>
       <c r="Y10" s="16"/>
     </row>
-    <row r="11" spans="1:25" ht="15.75" customHeight="1">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1520</v>
       </c>
@@ -18840,7 +18840,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1">
+    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1521</v>
       </c>
@@ -18870,7 +18870,7 @@
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1">
+    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1522</v>
       </c>
@@ -18969,17 +18969,17 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="3" customWidth="1"/>
-    <col min="3" max="23" width="9.140625" style="3"/>
-    <col min="24" max="24" width="8.5703125" style="3" customWidth="1"/>
-    <col min="25" max="25" width="45.140625" style="3" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="15.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="3" customWidth="1"/>
+    <col min="3" max="23" width="9.1640625" style="3"/>
+    <col min="24" max="24" width="8.5" style="3" customWidth="1"/>
+    <col min="25" max="25" width="45.1640625" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -19056,7 +19056,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" customHeight="1">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1279</v>
       </c>
@@ -19064,7 +19064,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="18.399999999999999" customHeight="1">
+    <row r="3" spans="1:30" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1281</v>
       </c>
@@ -19072,11 +19072,11 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="12.75" customHeight="1">
+    <row r="4" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1517</v>
       </c>
@@ -19084,7 +19084,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="85.5">
+    <row r="6" spans="1:30" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1518</v>
       </c>
@@ -19092,13 +19092,13 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:30" customFormat="1">
+    <row r="9" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>838</v>
       </c>
@@ -19180,7 +19180,7 @@
       <c r="AC9" s="27"/>
       <c r="AD9" s="27"/>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1533</v>
       </c>
@@ -19188,7 +19188,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1535</v>
       </c>
@@ -19265,7 +19265,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1560</v>
       </c>
@@ -19342,7 +19342,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1585</v>
       </c>
@@ -19419,7 +19419,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1609</v>
       </c>
@@ -19496,7 +19496,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1633</v>
       </c>
@@ -19573,7 +19573,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1658</v>
       </c>
@@ -19650,7 +19650,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1682</v>
       </c>
@@ -19727,7 +19727,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1706</v>
       </c>
@@ -19804,7 +19804,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1730</v>
       </c>
@@ -19881,7 +19881,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1754</v>
       </c>
@@ -19958,7 +19958,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1778</v>
       </c>
@@ -20035,7 +20035,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1802</v>
       </c>
@@ -20112,7 +20112,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1827</v>
       </c>
@@ -20189,7 +20189,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1851</v>
       </c>
@@ -20266,7 +20266,7 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1875</v>
       </c>
@@ -20343,7 +20343,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1899</v>
       </c>
@@ -20420,7 +20420,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1923</v>
       </c>
@@ -20497,7 +20497,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1947</v>
       </c>
@@ -20574,7 +20574,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1971</v>
       </c>
@@ -20651,7 +20651,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1995</v>
       </c>
@@ -20728,7 +20728,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2019</v>
       </c>
@@ -20805,7 +20805,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2043</v>
       </c>
@@ -20882,7 +20882,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2067</v>
       </c>
@@ -20959,7 +20959,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2091</v>
       </c>
@@ -21036,7 +21036,7 @@
         <v>2114</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>2115</v>
       </c>
@@ -21113,7 +21113,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>2139</v>
       </c>
@@ -21190,7 +21190,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>2163</v>
       </c>
@@ -21935,13 +21935,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="17" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="3" max="17" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -22018,7 +22018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2187</v>
       </c>
@@ -22095,7 +22095,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2205</v>
       </c>
@@ -22172,7 +22172,7 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2221</v>
       </c>
@@ -22249,7 +22249,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2238</v>
       </c>
@@ -22326,7 +22326,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2261</v>
       </c>
@@ -22403,7 +22403,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2282</v>
       </c>
@@ -22480,7 +22480,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2305</v>
       </c>
@@ -22557,7 +22557,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2326</v>
       </c>
@@ -22634,7 +22634,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2343</v>
       </c>
@@ -22711,7 +22711,7 @@
         <v>2344</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2362</v>
       </c>
@@ -22788,7 +22788,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2384</v>
       </c>
@@ -22865,7 +22865,7 @@
         <v>2388</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2407</v>
       </c>
@@ -22942,7 +22942,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2430</v>
       </c>
@@ -23019,7 +23019,7 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2453</v>
       </c>
@@ -23096,7 +23096,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2472</v>
       </c>
@@ -23173,7 +23173,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2490</v>
       </c>
@@ -23250,7 +23250,7 @@
         <v>2495</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2507</v>
       </c>
@@ -23327,7 +23327,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2524</v>
       </c>
@@ -23404,7 +23404,7 @@
         <v>2528</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2538</v>
       </c>
@@ -23481,7 +23481,7 @@
         <v>2539</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2544</v>
       </c>
@@ -23558,7 +23558,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2567</v>
       </c>
@@ -23635,7 +23635,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2586</v>
       </c>
@@ -23712,7 +23712,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2600</v>
       </c>
@@ -23789,7 +23789,7 @@
         <v>2605</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2621</v>
       </c>
@@ -23866,7 +23866,7 @@
         <v>2643</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2644</v>
       </c>
@@ -23943,7 +23943,7 @@
         <v>2648</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2664</v>
       </c>
@@ -24020,7 +24020,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2687</v>
       </c>
@@ -24103,12 +24103,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d5d883e-0c28-478a-ac53-9f06c055995e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d" xsi:nil="true"/>
+    <SharedWithUsers xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d">
+      <UserInfo>
+        <DisplayName>BELOSINSCHI Irina-Elena</DisplayName>
+        <AccountId>47</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24335,31 +24344,48 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d5d883e-0c28-478a-ac53-9f06c055995e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d" xsi:nil="true"/>
-    <SharedWithUsers xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d">
-      <UserInfo>
-        <DisplayName>BELOSINSCHI Irina-Elena</DisplayName>
-        <AccountId>47</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7D1253-D834-493E-9026-071E0E5EAEC3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6341A026-459C-4E5E-A4F6-A3C41C470367}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6d5d883e-0c28-478a-ac53-9f06c055995e"/>
+    <ds:schemaRef ds:uri="00415896-3eb3-49ce-a9f9-9a4c063fc79d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6622F560-A171-4B5B-BCDE-C82BD09D9C77}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6622F560-A171-4B5B-BCDE-C82BD09D9C77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00415896-3eb3-49ce-a9f9-9a4c063fc79d"/>
+    <ds:schemaRef ds:uri="6d5d883e-0c28-478a-ac53-9f06c055995e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6341A026-459C-4E5E-A4F6-A3C41C470367}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7D1253-D834-493E-9026-071E0E5EAEC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Corrections on multiple languages
https://ep-jira-issue-tracking.in.ep.europa.eu/ep-jira/browse/NARRATIO-852
</commit_message>
<xml_diff>
--- a/_imports/MFFContent.xlsx
+++ b/_imports/MFFContent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbraga\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{397A4D49-B1EA-4656-B6C0-06A6784B3C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AECFBF1-835F-466D-9738-643EDC851B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -7760,7 +7760,7 @@
 Los desafíos comunes de Europa se abordan mejor en conjunto. El presupuesto de la UE a largo plazo aporta un valor añadido europeo al combinar recursos, lo que permite financiar proyectos y políticas que resultan más eficientes si se llevan a cabo conjuntamente en lugar de forma individual.
 En los últimos años, el contexto político, económico y social ha cambiado notablemente. Hoy en día, la agresión de Rusia contra Ucrania, la necesidad de que la UE siga siendo competitiva, el apoyo a las empresas en la transformación digital y la lucha contra el cambio climático suponen grandes desafíos para la seguridad y la economía europeas.
 Ahora, la UE debe decidir sobre un presupuesto de la UE a largo plazo que respalde la economía y las sociedades europeas a partir de 2028. El contexto sigue siendo extremadamente exigente. Hay **realidades difíciles que no podemos ignorar**: la guerra en Ucrania, el alto coste de la vida, la necesidad de reforzar nuestra seguridad y competitividad, y el reto del cambio climático. Europa debe **invertir en lo que importa**.
-[Las encuestas del Eurobarómetro muestran] (https://europa.eu/eurobarometer/surveys/detail/3492?etrans=es) que los europeos esperan una actuación clara de la UE en varias áreas clave: economía y asuntos sociales, defensa y seguridad, cambio climático y agricultura.
+[Las encuestas del Eurobarómetro muestran](https://europa.eu/eurobarometer/surveys/detail/3492?etrans=es) que los europeos esperan una actuación clara de la UE en varias áreas clave: economía y asuntos sociales, defensa y seguridad, cambio climático y agricultura.
 El Parlamento Europeo trabaja junto con las demás instituciones de la UE para responder a estas expectativas y definir el próximo presupuesto de la UE a largo plazo.</t>
   </si>
   <si>
@@ -9822,9 +9822,9 @@
 Rozpočet slouží 450 milionům obyvatel a představuje malou část celkových veřejných výdajů v EU. Je například menší než státní rozpočet Rakouska (9 milionů obyvatel): pro rok 2022 [činil rozpočet EU přibližně 170 miliard eur](https://commission.europa.eu/strategy-and-policy/eu-budget/annual-eu-budget/all-annual-budgets/2022_en?prefLang=cs) a [rozpočet Rakouska činil přibližně 240 miliard eur](https://ec.europa.eu/eurostat/databrowser/view/gov_10a_exp__custom_13928345/default/table?lang=en).</t>
   </si>
   <si>
-    <t xml:space="preserve">EU's budget er relativt lille sammenlignet med de nationale budgetter. Det udgør årligt ca. 1 % af EU's BNI (bruttonationalindkomst) eller ca. 160-180 mia. EUR. De nationale offentlige udgifter i EU-landene udgør i gennemsnit næsten 50 % af deres respektive BNI.
+    <t xml:space="preserve">EU's budget er relativt lille sammenlignet med de nationale budgetter. Det udgør årligt ca. [1 % af EU's BNI (bruttonationalindkomst)](https://www.eca.europa.eu/da/the-eu-finances) eller ca. 160-180 mia. EUR. De nationale offentlige udgifter i EU-landene udgør i gennemsnit næsten 50 % af deres respektive BNI.
 I henhold til det nuværende langsigtede EU-budget kan EU forpligte sig til at bruge 1074 mia. euro (i 2018-priser) mellem 2021 og 2027.
-Budgettet er til gavn for 450 millioner indbyggere og udgør en lille del af de samlede offentlige udgifter i EU. Det er f.eks. mindre end det nationale budget i Østrig (9 millioner indbyggere): For 2022 var EU's budget på ca. 170 mia. EUR, mens det østrigske nationale budget var på ca. 240 mia. EUR.
+Budgettet er til gavn for 450 millioner indbyggere og udgør en lille del af de samlede offentlige udgifter i EU. Det er f.eks. mindre end det nationale budget i Østrig (9 millioner indbyggere): For 2022 var [EU's budget på ca. 170 mia. EUR](https://commission.europa.eu/strategy-and-policy/eu-budget/annual-eu-budget/all-annual-budgets/2022_en), mens [det østrigske nationale budget var på ca. 240 mia. EUR](https://ec.europa.eu/eurostat/databrowser/view/gov_10a_exp__custom_13928345/default/table?lang=en).
 </t>
   </si>
   <si>
@@ -9880,9 +9880,9 @@
 Il bilancio riguarda 450 milioni di cittadini e rappresenta una piccola percentuale della spesa pubblica complessiva dell'UE. A titolo di esempio, è inferiore al bilancio nazionale dell'Austria (9 milioni di abitanti): per il 2022, [il bilancio dell'UE era di circa 170 miliardi di euro](https://commission.europa. eu/strategy-and-policy/eu-budget/annual-eu-budget/all-annual-budgets/2022_en), mentre [il bilancio nazionale austriaco era di circa 240 miliardi di euro](https://ec.europa.eu/eurostat/databrowser/view/gov_10a_exp__custom_13928345/default/table?lang=en).</t>
   </si>
   <si>
-    <t xml:space="preserve">ES biudžetas, palyginti su nacionaliniais biudžetais, yra nedidelis. Kasmet jis sudaro apie [1 proc. ES BNP] (https://www.eca.europa.eu/lt/the-eu-finances) (bendrųjų nacionalinių pajamų), t. y. apie 160–180 mlrd. eurų. ES šalių nacionalinės viešosios išlaidos vidutiniškai sudaro beveik 50 proc. jų atitinkamų BNP.
+    <t xml:space="preserve">ES biudžetas, palyginti su nacionaliniais biudžetais, yra nedidelis. Kasmet jis sudaro apie [1 proc. ES BNP](https://www.eca.europa.eu/lt/the-eu-finances) (bendrųjų nacionalinių pajamų), t. y. apie 160–180 mlrd. eurų. ES šalių nacionalinės viešosios išlaidos vidutiniškai sudaro beveik 50 proc. jų atitinkamų BNP.
 Pagal dabartinį ES daugiametį biudžetą 2021–2027 m. ES gali įsipareigoti išleisti 1 074 mlrd. eurų (2018 m. kainomis).
-Šis biudžetas skirtas 450 mln. gyventojų ir sudaro nedidelę visų ES viešųjų išlaidų dalį. Pavyzdžiui, jis yra mažesnis už Austrijos (9 mln. gyventojų) nacionalinį biudžetą: 2022 m. [ES biudžetas sudarė apie 170 mlrd. eurų] (https://commission.europa.eu/strategy-and-policy/eu-budget/annual-eu-budget/all-annual-budgets/2022_en?prefLang=lt), o Austrijos nacionalinis biudžetas – apie 240 mlrd. eurų.
+Šis biudžetas skirtas 450 mln. gyventojų ir sudaro nedidelę visų ES viešųjų išlaidų dalį. Pavyzdžiui, jis yra mažesnis už Austrijos (9 mln. gyventojų) nacionalinį biudžetą: 2022 m. [ES biudžetas sudarė apie 170 mlrd. eurų](https://commission.europa.eu/strategy-and-policy/eu-budget/annual-eu-budget/all-annual-budgets/2022_en?prefLang=lt), o [Austrijos nacionalinis biudžetas – apie 240 mlrd. eurų](https://ec.europa.eu/eurostat/databrowser/view/gov_10a_exp__custom_13928345/default/table?lang=en).
 </t>
   </si>
   <si>
@@ -17043,7 +17043,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17204,9 +17204,6 @@
     <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -19295,7 +19292,7 @@
   <dimension ref="A1:CZ73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="B66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -24577,12 +24574,12 @@
       <c r="Y68" s="66" t="s">
         <v>1507</v>
       </c>
-      <c r="Z68" s="79"/>
-      <c r="AA68" s="79"/>
-      <c r="AB68" s="79"/>
-      <c r="AC68" s="79"/>
-      <c r="AD68" s="79"/>
-      <c r="AE68" s="79"/>
+      <c r="Z68" s="78"/>
+      <c r="AA68" s="78"/>
+      <c r="AB68" s="78"/>
+      <c r="AC68" s="78"/>
+      <c r="AD68" s="78"/>
+      <c r="AE68" s="78"/>
     </row>
     <row r="69" spans="1:31" s="67" customFormat="1">
       <c r="A69" s="32" t="s">
@@ -24660,12 +24657,12 @@
       <c r="Y69" s="66" t="s">
         <v>1532</v>
       </c>
-      <c r="Z69" s="79"/>
-      <c r="AA69" s="79"/>
-      <c r="AB69" s="79"/>
-      <c r="AC69" s="79"/>
-      <c r="AD69" s="79"/>
-      <c r="AE69" s="79"/>
+      <c r="Z69" s="78"/>
+      <c r="AA69" s="78"/>
+      <c r="AB69" s="78"/>
+      <c r="AC69" s="78"/>
+      <c r="AD69" s="78"/>
+      <c r="AE69" s="78"/>
     </row>
     <row r="70" spans="1:31" s="67" customFormat="1">
       <c r="A70" s="32"/>
@@ -24693,12 +24690,12 @@
       <c r="W70" s="66"/>
       <c r="X70" s="66"/>
       <c r="Y70" s="66"/>
-      <c r="Z70" s="79"/>
-      <c r="AA70" s="79"/>
-      <c r="AB70" s="79"/>
-      <c r="AC70" s="79"/>
-      <c r="AD70" s="79"/>
-      <c r="AE70" s="79"/>
+      <c r="Z70" s="78"/>
+      <c r="AA70" s="78"/>
+      <c r="AB70" s="78"/>
+      <c r="AC70" s="78"/>
+      <c r="AD70" s="78"/>
+      <c r="AE70" s="78"/>
     </row>
     <row r="71" spans="1:31" s="67" customFormat="1">
       <c r="A71" s="32" t="s">
@@ -24776,12 +24773,12 @@
       <c r="Y71" s="66" t="s">
         <v>1555</v>
       </c>
-      <c r="Z71" s="79"/>
-      <c r="AA71" s="79"/>
-      <c r="AB71" s="79"/>
-      <c r="AC71" s="79"/>
-      <c r="AD71" s="79"/>
-      <c r="AE71" s="79"/>
+      <c r="Z71" s="78"/>
+      <c r="AA71" s="78"/>
+      <c r="AB71" s="78"/>
+      <c r="AC71" s="78"/>
+      <c r="AD71" s="78"/>
+      <c r="AE71" s="78"/>
     </row>
     <row r="72" spans="1:31">
       <c r="A72" t="s">
@@ -25038,7 +25035,7 @@
   <dimension ref="A1:Z66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -25992,76 +25989,76 @@
       <c r="B18" s="3" t="s">
         <v>1800</v>
       </c>
-      <c r="C18" s="79" t="s">
+      <c r="C18" s="78" t="s">
         <v>1801</v>
       </c>
-      <c r="D18" s="79" t="s">
+      <c r="D18" s="78" t="s">
         <v>1802</v>
       </c>
-      <c r="E18" s="79" t="s">
+      <c r="E18" s="78" t="s">
         <v>1803</v>
       </c>
-      <c r="F18" s="79" t="s">
+      <c r="F18" s="78" t="s">
         <v>1804</v>
       </c>
-      <c r="G18" s="79" t="s">
+      <c r="G18" s="78" t="s">
         <v>1805</v>
       </c>
-      <c r="H18" s="79" t="s">
+      <c r="H18" s="78" t="s">
         <v>1806</v>
       </c>
-      <c r="I18" s="79" t="s">
+      <c r="I18" s="78" t="s">
         <v>1807</v>
       </c>
-      <c r="J18" s="79" t="s">
+      <c r="J18" s="78" t="s">
         <v>1808</v>
       </c>
-      <c r="K18" s="79" t="s">
+      <c r="K18" s="78" t="s">
         <v>1809</v>
       </c>
-      <c r="L18" s="79" t="s">
+      <c r="L18" s="78" t="s">
         <v>1810</v>
       </c>
-      <c r="M18" s="79" t="s">
+      <c r="M18" s="78" t="s">
         <v>1811</v>
       </c>
-      <c r="N18" s="79" t="s">
+      <c r="N18" s="78" t="s">
         <v>1812</v>
       </c>
-      <c r="O18" s="79" t="s">
+      <c r="O18" s="78" t="s">
         <v>1813</v>
       </c>
-      <c r="P18" s="79" t="s">
+      <c r="P18" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="Q18" s="79" t="s">
+      <c r="Q18" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="R18" s="79" t="s">
+      <c r="R18" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="79" t="s">
+      <c r="S18" s="78" t="s">
         <v>1814</v>
       </c>
-      <c r="T18" s="79" t="s">
+      <c r="T18" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="U18" s="79" t="s">
+      <c r="U18" s="78" t="s">
         <v>1815</v>
       </c>
-      <c r="V18" s="79" t="s">
+      <c r="V18" s="78" t="s">
         <v>1816</v>
       </c>
-      <c r="W18" s="79" t="s">
+      <c r="W18" s="78" t="s">
         <v>1817</v>
       </c>
-      <c r="X18" s="79" t="s">
+      <c r="X18" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="Y18" s="79" t="s">
+      <c r="Y18" s="78" t="s">
         <v>1818</v>
       </c>
-      <c r="Z18" s="79"/>
+      <c r="Z18" s="78"/>
     </row>
     <row r="19" spans="1:26" s="44" customFormat="1" ht="30.75">
       <c r="A19" s="12" t="s">
@@ -26139,7 +26136,7 @@
       <c r="Y19" s="10" t="s">
         <v>1842</v>
       </c>
-      <c r="Z19" s="79"/>
+      <c r="Z19" s="78"/>
     </row>
     <row r="20" spans="1:26" s="44" customFormat="1" ht="15">
       <c r="A20" s="12" t="s">
@@ -26217,7 +26214,7 @@
       <c r="Y20" s="14" t="s">
         <v>1866</v>
       </c>
-      <c r="Z20" s="79"/>
+      <c r="Z20" s="78"/>
     </row>
     <row r="21" spans="1:26">
       <c r="B21" s="14"/>
@@ -28780,9 +28777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="C2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
@@ -29205,7 +29202,7 @@
       <c r="G7" s="3" t="s">
         <v>2539</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="7" t="s">
         <v>2540</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -29447,8 +29444,8 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
@@ -31864,13 +31861,13 @@
       <c r="D34" s="7" t="s">
         <v>3007</v>
       </c>
-      <c r="E34" s="77" t="s">
+      <c r="E34" s="76" t="s">
         <v>3008</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>3009</v>
       </c>
-      <c r="G34" s="78" t="s">
+      <c r="G34" s="77" t="s">
         <v>3010</v>
       </c>
       <c r="H34" s="3" t="s">
@@ -32303,7 +32300,7 @@
       <c r="V39" s="7" t="s">
         <v>3098</v>
       </c>
-      <c r="W39" s="78" t="s">
+      <c r="W39" s="77" t="s">
         <v>3099</v>
       </c>
       <c r="X39" s="7" t="s">
@@ -33448,9 +33445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20:Y20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="12.75" customHeight="1"/>
@@ -34385,7 +34382,7 @@
       <c r="X14" s="7" t="s">
         <v>3468</v>
       </c>
-      <c r="Y14" s="77" t="s">
+      <c r="Y14" s="76" t="s">
         <v>3469</v>
       </c>
     </row>
@@ -41107,33 +41104,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d5d883e-0c28-478a-ac53-9f06c055995e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d" xsi:nil="true"/>
-    <SharedWithUsers xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d">
-      <UserInfo>
-        <DisplayName>BELOSINSCHI Irina-Elena</DisplayName>
-        <AccountId>47</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038C918D8E59A1B44AAEA5DD61DCD4207" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1055e28e48ff09895739331c5007bec3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00415896-3eb3-49ce-a9f9-9a4c063fc79d" xmlns:ns3="6d5d883e-0c28-478a-ac53-9f06c055995e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e55e4adc7e9f7d8b664df317583a40fd" ns2:_="" ns3:_="">
     <xsd:import namespace="00415896-3eb3-49ce-a9f9-9a4c063fc79d"/>
@@ -41356,8 +41326,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d5d883e-0c28-478a-ac53-9f06c055995e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d" xsi:nil="true"/>
+    <SharedWithUsers xmlns="00415896-3eb3-49ce-a9f9-9a4c063fc79d">
+      <UserInfo>
+        <DisplayName>BELOSINSCHI Irina-Elena</DisplayName>
+        <AccountId>47</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7D1253-D834-493E-9026-071E0E5EAEC3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6622F560-A171-4B5B-BCDE-C82BD09D9C77}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -41365,5 +41362,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6622F560-A171-4B5B-BCDE-C82BD09D9C77}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF7D1253-D834-493E-9026-071E0E5EAEC3}"/>
 </file>
</xml_diff>